<commit_message>
added project files final
</commit_message>
<xml_diff>
--- a/public/clients.xlsx
+++ b/public/clients.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>CLIENT_ID</t>
   </si>
@@ -24,6 +24,192 @@
   </si>
   <si>
     <t>CUSTOMER_ID</t>
+  </si>
+  <si>
+    <t>Transdigm</t>
+  </si>
+  <si>
+    <t>Wabtec</t>
+  </si>
+  <si>
+    <t>Valeo</t>
+  </si>
+  <si>
+    <t>Trane (Quest-CHN)</t>
+  </si>
+  <si>
+    <t>Trane (Quest-BLR)</t>
+  </si>
+  <si>
+    <t>TATA Hitachi</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>Tecnicas Reunidas</t>
+  </si>
+  <si>
+    <t>Technip (Quest-HYD)</t>
+  </si>
+  <si>
+    <t>Technip (Quest-CHN)</t>
+  </si>
+  <si>
+    <t>Synapse</t>
+  </si>
+  <si>
+    <t>Sumedhas Tech</t>
+  </si>
+  <si>
+    <t>Siemens</t>
+  </si>
+  <si>
+    <t>SECO</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>Rockwell</t>
+  </si>
+  <si>
+    <t>RJIO</t>
+  </si>
+  <si>
+    <t>Quest-Informatics</t>
+  </si>
+  <si>
+    <t>Quest-HYD</t>
+  </si>
+  <si>
+    <t>Quest-CHN</t>
+  </si>
+  <si>
+    <t>Quest-BLR</t>
+  </si>
+  <si>
+    <t>PSA</t>
+  </si>
+  <si>
+    <t>Plastic Omnium</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>Oceaneering</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Michelin</t>
+  </si>
+  <si>
+    <t>MBRDI</t>
+  </si>
+  <si>
+    <t>Lear</t>
+  </si>
+  <si>
+    <t>John Deere</t>
+  </si>
+  <si>
+    <t>Inteva</t>
+  </si>
+  <si>
+    <t>Ingersoll Rand</t>
+  </si>
+  <si>
+    <t>Inspirisys</t>
+  </si>
+  <si>
+    <t>Ibhaan</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>HPE</t>
+  </si>
+  <si>
+    <t>Honeywell</t>
+  </si>
+  <si>
+    <t>Hitachi</t>
+  </si>
+  <si>
+    <t>HCL</t>
+  </si>
+  <si>
+    <t>Halliburton</t>
+  </si>
+  <si>
+    <t>H&amp;R Block</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>Garrett Motion</t>
+  </si>
+  <si>
+    <t>Fourbricks</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>FCA</t>
+  </si>
+  <si>
+    <t>Exxonmobil</t>
+  </si>
+  <si>
+    <t>Envision</t>
+  </si>
+  <si>
+    <t>DTICI</t>
+  </si>
+  <si>
+    <t>Dover</t>
+  </si>
+  <si>
+    <t>Collins</t>
+  </si>
+  <si>
+    <t>Caterpillar</t>
+  </si>
+  <si>
+    <t>Boeing</t>
+  </si>
+  <si>
+    <t>Baxter</t>
+  </si>
+  <si>
+    <t>Baker Huges</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>ASACO</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Analytic Edge</t>
+  </si>
+  <si>
+    <t>Alstom</t>
+  </si>
+  <si>
+    <t>Airbus</t>
+  </si>
+  <si>
+    <t>ABB</t>
   </si>
 </sst>
 </file>
@@ -359,7 +545,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,6 +562,688 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>12</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>11</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>